<commit_message>
fix contact, update invoice
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/Invoice.xlsx
+++ b/lib/PHPExcel/templates/Invoice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GPM\www\GPM-TEST\lib\PHPExcel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\lib\PHPExcel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B160344-FF3F-49FE-AF0C-451838BF021D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2C31ED-F975-4968-83DE-FD865181BDC7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="9195" windowHeight="5460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,20 +18,20 @@
     <sheet name="Template" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database" localSheetId="1">InvoiceUSA!$A$13:$G$48</definedName>
+    <definedName name="_xlnm.Database" localSheetId="1">InvoiceUSA!$A$14:$G$49</definedName>
     <definedName name="_xlnm.Database" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Database">InvoiceFR!$A$13:$G$48</definedName>
+    <definedName name="_xlnm.Database">InvoiceFR!$A$14:$G$49</definedName>
     <definedName name="_xlnm.Data_Form" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Data_Form">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">InvoiceFR!$A$1:$G$53</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">InvoiceUSA!$A$1:$G$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">InvoiceFR!$A$1:$G$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">InvoiceUSA!$A$1:$G$54</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>:</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>V.A.T. 20 %</t>
+  </si>
+  <si>
+    <t>Référence Client</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
     <xf numFmtId="40" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,9 +535,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -576,7 +579,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -668,7 +682,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>419101</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>97221</xdr:rowOff>
     </xdr:to>
@@ -734,7 +748,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>97221</xdr:rowOff>
     </xdr:to>
@@ -1110,18 +1124,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K182"/>
+  <sheetPr codeName="Feuil1"/>
+  <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="2.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
@@ -1145,10 +1160,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H3" s="20"/>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="52" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1175,7 +1190,7 @@
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="61"/>
       <c r="I6" s="11" t="s">
         <v>45</v>
       </c>
@@ -1190,7 +1205,7 @@
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="60"/>
       <c r="I7" s="11" t="s">
         <v>43</v>
       </c>
@@ -1204,10 +1219,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="52" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1245,390 +1260,391 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B13" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G13" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
+    <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="16"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="14"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
+      <c r="A16" s="59"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="52"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="16"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="52"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="16"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
+      <c r="A20" s="59"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="16"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="16"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="52"/>
+      <c r="G21" s="51"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
+    <row r="22" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="59"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="16"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="14"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="16"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
       <c r="E25" s="16"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="59"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="16"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="59"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="16"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="52"/>
+      <c r="G27" s="51"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="16"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="52"/>
+      <c r="G28" s="51"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="16"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="52"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="15"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="16"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="52"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
       <c r="E32" s="16"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="52"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="59"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="16"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="52"/>
+      <c r="G33" s="51"/>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="59"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="16"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="52"/>
+      <c r="G34" s="51"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="59"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="52"/>
+      <c r="G35" s="51"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="59"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="52"/>
+      <c r="G36" s="51"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="59"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="52"/>
+      <c r="G37" s="51"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="59"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="52"/>
+      <c r="G38" s="51"/>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="16"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="52"/>
+      <c r="G39" s="51"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="16"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="52"/>
+      <c r="G40" s="51"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="16"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G41" s="51"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="16"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="52"/>
+      <c r="G42" s="51"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="16"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="52"/>
-    </row>
-    <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G43" s="51"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="16"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G44" s="51"/>
+    </row>
+    <row r="45" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="16"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="52"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G45" s="51"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="16"/>
       <c r="F46" s="7"/>
-      <c r="G46" s="52"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G46" s="51"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="16"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="52"/>
-    </row>
-    <row r="48" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G47" s="51"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="16"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G48" s="51"/>
+    </row>
+    <row r="49" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="16"/>
       <c r="F49" s="7"/>
-      <c r="G49" s="52"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
@@ -1637,8 +1653,7 @@
       <c r="D50" s="18"/>
       <c r="E50" s="16"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="52"/>
-      <c r="I50" s="10"/>
+      <c r="G50" s="51"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="18"/>
@@ -1647,7 +1662,8 @@
       <c r="D51" s="18"/>
       <c r="E51" s="16"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="52"/>
+      <c r="G51" s="51"/>
+      <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
@@ -1656,7 +1672,7 @@
       <c r="D52" s="18"/>
       <c r="E52" s="16"/>
       <c r="F52" s="7"/>
-      <c r="G52" s="52"/>
+      <c r="G52" s="51"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
@@ -1665,18 +1681,16 @@
       <c r="D53" s="18"/>
       <c r="E53" s="16"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="52"/>
-    </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G53" s="51"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
       <c r="E54" s="16"/>
       <c r="F54" s="7"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="1"/>
+      <c r="G54" s="51"/>
     </row>
     <row r="55" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18"/>
@@ -1685,19 +1699,20 @@
       <c r="D55" s="18"/>
       <c r="E55" s="16"/>
       <c r="F55" s="7"/>
-      <c r="G55" s="52"/>
+      <c r="G55" s="51"/>
       <c r="H55" s="12"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
       <c r="E56" s="16"/>
       <c r="F56" s="7"/>
-      <c r="G56" s="52"/>
-      <c r="I56" s="10"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
@@ -1706,7 +1721,7 @@
       <c r="D57" s="18"/>
       <c r="E57" s="16"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="52"/>
+      <c r="G57" s="51"/>
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -1716,7 +1731,8 @@
       <c r="D58" s="18"/>
       <c r="E58" s="16"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="52"/>
+      <c r="G58" s="51"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="18"/>
@@ -1725,7 +1741,7 @@
       <c r="D59" s="18"/>
       <c r="E59" s="16"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="52"/>
+      <c r="G59" s="51"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="18"/>
@@ -1734,7 +1750,7 @@
       <c r="D60" s="18"/>
       <c r="E60" s="16"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="52"/>
+      <c r="G60" s="51"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="18"/>
@@ -1743,7 +1759,7 @@
       <c r="D61" s="18"/>
       <c r="E61" s="16"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="52"/>
+      <c r="G61" s="51"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="18"/>
@@ -1752,7 +1768,7 @@
       <c r="D62" s="18"/>
       <c r="E62" s="16"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="52"/>
+      <c r="G62" s="51"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="18"/>
@@ -1761,7 +1777,7 @@
       <c r="D63" s="18"/>
       <c r="E63" s="16"/>
       <c r="F63" s="7"/>
-      <c r="G63" s="52"/>
+      <c r="G63" s="51"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="18"/>
@@ -1770,7 +1786,7 @@
       <c r="D64" s="18"/>
       <c r="E64" s="16"/>
       <c r="F64" s="7"/>
-      <c r="G64" s="52"/>
+      <c r="G64" s="51"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="18"/>
@@ -1779,7 +1795,7 @@
       <c r="D65" s="18"/>
       <c r="E65" s="16"/>
       <c r="F65" s="7"/>
-      <c r="G65" s="52"/>
+      <c r="G65" s="51"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="18"/>
@@ -1788,7 +1804,7 @@
       <c r="D66" s="18"/>
       <c r="E66" s="16"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="52"/>
+      <c r="G66" s="51"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="18"/>
@@ -1797,7 +1813,7 @@
       <c r="D67" s="18"/>
       <c r="E67" s="16"/>
       <c r="F67" s="7"/>
-      <c r="G67" s="52"/>
+      <c r="G67" s="51"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="18"/>
@@ -1806,7 +1822,7 @@
       <c r="D68" s="18"/>
       <c r="E68" s="16"/>
       <c r="F68" s="7"/>
-      <c r="G68" s="52"/>
+      <c r="G68" s="51"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="18"/>
@@ -1815,7 +1831,7 @@
       <c r="D69" s="18"/>
       <c r="E69" s="16"/>
       <c r="F69" s="7"/>
-      <c r="G69" s="52"/>
+      <c r="G69" s="51"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="18"/>
@@ -1824,7 +1840,7 @@
       <c r="D70" s="18"/>
       <c r="E70" s="16"/>
       <c r="F70" s="7"/>
-      <c r="G70" s="52"/>
+      <c r="G70" s="51"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="18"/>
@@ -1833,7 +1849,7 @@
       <c r="D71" s="18"/>
       <c r="E71" s="16"/>
       <c r="F71" s="7"/>
-      <c r="G71" s="52"/>
+      <c r="G71" s="51"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="18"/>
@@ -1842,7 +1858,7 @@
       <c r="D72" s="18"/>
       <c r="E72" s="16"/>
       <c r="F72" s="7"/>
-      <c r="G72" s="52"/>
+      <c r="G72" s="51"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="18"/>
@@ -1851,7 +1867,7 @@
       <c r="D73" s="18"/>
       <c r="E73" s="16"/>
       <c r="F73" s="7"/>
-      <c r="G73" s="52"/>
+      <c r="G73" s="51"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="18"/>
@@ -1860,7 +1876,7 @@
       <c r="D74" s="18"/>
       <c r="E74" s="16"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="52"/>
+      <c r="G74" s="51"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="18"/>
@@ -1869,7 +1885,7 @@
       <c r="D75" s="18"/>
       <c r="E75" s="16"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="52"/>
+      <c r="G75" s="51"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="18"/>
@@ -1878,7 +1894,7 @@
       <c r="D76" s="18"/>
       <c r="E76" s="16"/>
       <c r="F76" s="7"/>
-      <c r="G76" s="52"/>
+      <c r="G76" s="51"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="18"/>
@@ -1887,7 +1903,7 @@
       <c r="D77" s="18"/>
       <c r="E77" s="16"/>
       <c r="F77" s="7"/>
-      <c r="G77" s="52"/>
+      <c r="G77" s="51"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="18"/>
@@ -1896,7 +1912,7 @@
       <c r="D78" s="18"/>
       <c r="E78" s="16"/>
       <c r="F78" s="7"/>
-      <c r="G78" s="52"/>
+      <c r="G78" s="51"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="18"/>
@@ -1905,7 +1921,7 @@
       <c r="D79" s="18"/>
       <c r="E79" s="16"/>
       <c r="F79" s="7"/>
-      <c r="G79" s="52"/>
+      <c r="G79" s="51"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="18"/>
@@ -1914,7 +1930,7 @@
       <c r="D80" s="18"/>
       <c r="E80" s="16"/>
       <c r="F80" s="7"/>
-      <c r="G80" s="52"/>
+      <c r="G80" s="51"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="18"/>
@@ -1923,7 +1939,7 @@
       <c r="D81" s="18"/>
       <c r="E81" s="16"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="52"/>
+      <c r="G81" s="51"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="18"/>
@@ -1932,7 +1948,7 @@
       <c r="D82" s="18"/>
       <c r="E82" s="16"/>
       <c r="F82" s="7"/>
-      <c r="G82" s="52"/>
+      <c r="G82" s="51"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="18"/>
@@ -1941,7 +1957,7 @@
       <c r="D83" s="18"/>
       <c r="E83" s="16"/>
       <c r="F83" s="7"/>
-      <c r="G83" s="52"/>
+      <c r="G83" s="51"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="18"/>
@@ -1950,7 +1966,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="16"/>
       <c r="F84" s="7"/>
-      <c r="G84" s="52"/>
+      <c r="G84" s="51"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="18"/>
@@ -1959,7 +1975,7 @@
       <c r="D85" s="18"/>
       <c r="E85" s="16"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="52"/>
+      <c r="G85" s="51"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="18"/>
@@ -1968,16 +1984,16 @@
       <c r="D86" s="18"/>
       <c r="E86" s="16"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="52"/>
+      <c r="G86" s="51"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
+      <c r="B87" s="18"/>
       <c r="C87" s="18"/>
       <c r="D87" s="18"/>
       <c r="E87" s="16"/>
       <c r="F87" s="7"/>
-      <c r="G87" s="52"/>
+      <c r="G87" s="51"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="18"/>
@@ -1986,7 +2002,7 @@
       <c r="D88" s="18"/>
       <c r="E88" s="16"/>
       <c r="F88" s="7"/>
-      <c r="G88" s="52"/>
+      <c r="G88" s="51"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="18"/>
@@ -1995,7 +2011,7 @@
       <c r="D89" s="18"/>
       <c r="E89" s="16"/>
       <c r="F89" s="7"/>
-      <c r="G89" s="52"/>
+      <c r="G89" s="51"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="18"/>
@@ -2004,7 +2020,7 @@
       <c r="D90" s="18"/>
       <c r="E90" s="16"/>
       <c r="F90" s="7"/>
-      <c r="G90" s="52"/>
+      <c r="G90" s="51"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="18"/>
@@ -2013,7 +2029,7 @@
       <c r="D91" s="18"/>
       <c r="E91" s="16"/>
       <c r="F91" s="7"/>
-      <c r="G91" s="52"/>
+      <c r="G91" s="51"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="18"/>
@@ -2022,7 +2038,7 @@
       <c r="D92" s="18"/>
       <c r="E92" s="16"/>
       <c r="F92" s="7"/>
-      <c r="G92" s="52"/>
+      <c r="G92" s="51"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="18"/>
@@ -2031,7 +2047,7 @@
       <c r="D93" s="18"/>
       <c r="E93" s="16"/>
       <c r="F93" s="7"/>
-      <c r="G93" s="52"/>
+      <c r="G93" s="51"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="18"/>
@@ -2040,7 +2056,7 @@
       <c r="D94" s="18"/>
       <c r="E94" s="16"/>
       <c r="F94" s="7"/>
-      <c r="G94" s="52"/>
+      <c r="G94" s="51"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="18"/>
@@ -2049,7 +2065,7 @@
       <c r="D95" s="18"/>
       <c r="E95" s="16"/>
       <c r="F95" s="7"/>
-      <c r="G95" s="52"/>
+      <c r="G95" s="51"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="18"/>
@@ -2058,7 +2074,7 @@
       <c r="D96" s="18"/>
       <c r="E96" s="16"/>
       <c r="F96" s="7"/>
-      <c r="G96" s="52"/>
+      <c r="G96" s="51"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="18"/>
@@ -2067,7 +2083,7 @@
       <c r="D97" s="18"/>
       <c r="E97" s="16"/>
       <c r="F97" s="7"/>
-      <c r="G97" s="52"/>
+      <c r="G97" s="51"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="18"/>
@@ -2076,7 +2092,7 @@
       <c r="D98" s="18"/>
       <c r="E98" s="16"/>
       <c r="F98" s="7"/>
-      <c r="G98" s="52"/>
+      <c r="G98" s="51"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="18"/>
@@ -2085,7 +2101,7 @@
       <c r="D99" s="18"/>
       <c r="E99" s="16"/>
       <c r="F99" s="7"/>
-      <c r="G99" s="52"/>
+      <c r="G99" s="51"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="18"/>
@@ -2094,7 +2110,7 @@
       <c r="D100" s="18"/>
       <c r="E100" s="16"/>
       <c r="F100" s="7"/>
-      <c r="G100" s="52"/>
+      <c r="G100" s="51"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="18"/>
@@ -2103,7 +2119,7 @@
       <c r="D101" s="18"/>
       <c r="E101" s="16"/>
       <c r="F101" s="7"/>
-      <c r="G101" s="52"/>
+      <c r="G101" s="51"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="18"/>
@@ -2112,7 +2128,7 @@
       <c r="D102" s="18"/>
       <c r="E102" s="16"/>
       <c r="F102" s="7"/>
-      <c r="G102" s="52"/>
+      <c r="G102" s="51"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="18"/>
@@ -2121,7 +2137,7 @@
       <c r="D103" s="18"/>
       <c r="E103" s="16"/>
       <c r="F103" s="7"/>
-      <c r="G103" s="52"/>
+      <c r="G103" s="51"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="18"/>
@@ -2130,7 +2146,7 @@
       <c r="D104" s="18"/>
       <c r="E104" s="16"/>
       <c r="F104" s="7"/>
-      <c r="G104" s="52"/>
+      <c r="G104" s="51"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="18"/>
@@ -2139,7 +2155,7 @@
       <c r="D105" s="18"/>
       <c r="E105" s="16"/>
       <c r="F105" s="7"/>
-      <c r="G105" s="52"/>
+      <c r="G105" s="51"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="18"/>
@@ -2148,7 +2164,7 @@
       <c r="D106" s="18"/>
       <c r="E106" s="16"/>
       <c r="F106" s="7"/>
-      <c r="G106" s="52"/>
+      <c r="G106" s="51"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="18"/>
@@ -2157,7 +2173,7 @@
       <c r="D107" s="18"/>
       <c r="E107" s="16"/>
       <c r="F107" s="7"/>
-      <c r="G107" s="52"/>
+      <c r="G107" s="51"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="18"/>
@@ -2166,7 +2182,7 @@
       <c r="D108" s="18"/>
       <c r="E108" s="16"/>
       <c r="F108" s="7"/>
-      <c r="G108" s="52"/>
+      <c r="G108" s="51"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="18"/>
@@ -2175,7 +2191,7 @@
       <c r="D109" s="18"/>
       <c r="E109" s="16"/>
       <c r="F109" s="7"/>
-      <c r="G109" s="52"/>
+      <c r="G109" s="51"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="18"/>
@@ -2184,7 +2200,7 @@
       <c r="D110" s="18"/>
       <c r="E110" s="16"/>
       <c r="F110" s="7"/>
-      <c r="G110" s="52"/>
+      <c r="G110" s="51"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="18"/>
@@ -2193,7 +2209,7 @@
       <c r="D111" s="18"/>
       <c r="E111" s="16"/>
       <c r="F111" s="7"/>
-      <c r="G111" s="52"/>
+      <c r="G111" s="51"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="18"/>
@@ -2202,7 +2218,7 @@
       <c r="D112" s="18"/>
       <c r="E112" s="16"/>
       <c r="F112" s="7"/>
-      <c r="G112" s="52"/>
+      <c r="G112" s="51"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="18"/>
@@ -2211,7 +2227,7 @@
       <c r="D113" s="18"/>
       <c r="E113" s="16"/>
       <c r="F113" s="7"/>
-      <c r="G113" s="52"/>
+      <c r="G113" s="51"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="18"/>
@@ -2220,7 +2236,7 @@
       <c r="D114" s="18"/>
       <c r="E114" s="16"/>
       <c r="F114" s="7"/>
-      <c r="G114" s="52"/>
+      <c r="G114" s="51"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="18"/>
@@ -2229,7 +2245,7 @@
       <c r="D115" s="18"/>
       <c r="E115" s="16"/>
       <c r="F115" s="7"/>
-      <c r="G115" s="52"/>
+      <c r="G115" s="51"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="18"/>
@@ -2238,7 +2254,7 @@
       <c r="D116" s="18"/>
       <c r="E116" s="16"/>
       <c r="F116" s="7"/>
-      <c r="G116" s="52"/>
+      <c r="G116" s="51"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="18"/>
@@ -2247,7 +2263,7 @@
       <c r="D117" s="18"/>
       <c r="E117" s="16"/>
       <c r="F117" s="7"/>
-      <c r="G117" s="52"/>
+      <c r="G117" s="51"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="18"/>
@@ -2256,7 +2272,7 @@
       <c r="D118" s="18"/>
       <c r="E118" s="16"/>
       <c r="F118" s="7"/>
-      <c r="G118" s="52"/>
+      <c r="G118" s="51"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="18"/>
@@ -2265,7 +2281,7 @@
       <c r="D119" s="18"/>
       <c r="E119" s="16"/>
       <c r="F119" s="7"/>
-      <c r="G119" s="52"/>
+      <c r="G119" s="51"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="18"/>
@@ -2274,7 +2290,7 @@
       <c r="D120" s="18"/>
       <c r="E120" s="16"/>
       <c r="F120" s="7"/>
-      <c r="G120" s="52"/>
+      <c r="G120" s="51"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="18"/>
@@ -2283,7 +2299,7 @@
       <c r="D121" s="18"/>
       <c r="E121" s="16"/>
       <c r="F121" s="7"/>
-      <c r="G121" s="52"/>
+      <c r="G121" s="51"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="18"/>
@@ -2292,7 +2308,7 @@
       <c r="D122" s="18"/>
       <c r="E122" s="16"/>
       <c r="F122" s="7"/>
-      <c r="G122" s="52"/>
+      <c r="G122" s="51"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="18"/>
@@ -2301,7 +2317,7 @@
       <c r="D123" s="18"/>
       <c r="E123" s="16"/>
       <c r="F123" s="7"/>
-      <c r="G123" s="52"/>
+      <c r="G123" s="51"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="18"/>
@@ -2310,7 +2326,7 @@
       <c r="D124" s="18"/>
       <c r="E124" s="16"/>
       <c r="F124" s="7"/>
-      <c r="G124" s="52"/>
+      <c r="G124" s="51"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="18"/>
@@ -2319,7 +2335,7 @@
       <c r="D125" s="18"/>
       <c r="E125" s="16"/>
       <c r="F125" s="7"/>
-      <c r="G125" s="52"/>
+      <c r="G125" s="51"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="18"/>
@@ -2328,7 +2344,7 @@
       <c r="D126" s="18"/>
       <c r="E126" s="16"/>
       <c r="F126" s="7"/>
-      <c r="G126" s="52"/>
+      <c r="G126" s="51"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="18"/>
@@ -2337,7 +2353,7 @@
       <c r="D127" s="18"/>
       <c r="E127" s="16"/>
       <c r="F127" s="7"/>
-      <c r="G127" s="52"/>
+      <c r="G127" s="51"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="18"/>
@@ -2346,7 +2362,7 @@
       <c r="D128" s="18"/>
       <c r="E128" s="16"/>
       <c r="F128" s="7"/>
-      <c r="G128" s="52"/>
+      <c r="G128" s="51"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="18"/>
@@ -2355,7 +2371,7 @@
       <c r="D129" s="18"/>
       <c r="E129" s="16"/>
       <c r="F129" s="7"/>
-      <c r="G129" s="52"/>
+      <c r="G129" s="51"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="18"/>
@@ -2364,7 +2380,7 @@
       <c r="D130" s="18"/>
       <c r="E130" s="16"/>
       <c r="F130" s="7"/>
-      <c r="G130" s="52"/>
+      <c r="G130" s="51"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="18"/>
@@ -2373,7 +2389,7 @@
       <c r="D131" s="18"/>
       <c r="E131" s="16"/>
       <c r="F131" s="7"/>
-      <c r="G131" s="52"/>
+      <c r="G131" s="51"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="18"/>
@@ -2382,7 +2398,7 @@
       <c r="D132" s="18"/>
       <c r="E132" s="16"/>
       <c r="F132" s="7"/>
-      <c r="G132" s="52"/>
+      <c r="G132" s="51"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="18"/>
@@ -2391,7 +2407,7 @@
       <c r="D133" s="18"/>
       <c r="E133" s="16"/>
       <c r="F133" s="7"/>
-      <c r="G133" s="52"/>
+      <c r="G133" s="51"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="18"/>
@@ -2400,7 +2416,7 @@
       <c r="D134" s="18"/>
       <c r="E134" s="16"/>
       <c r="F134" s="7"/>
-      <c r="G134" s="52"/>
+      <c r="G134" s="51"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="18"/>
@@ -2409,7 +2425,7 @@
       <c r="D135" s="18"/>
       <c r="E135" s="16"/>
       <c r="F135" s="7"/>
-      <c r="G135" s="52"/>
+      <c r="G135" s="51"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="18"/>
@@ -2418,7 +2434,7 @@
       <c r="D136" s="18"/>
       <c r="E136" s="16"/>
       <c r="F136" s="7"/>
-      <c r="G136" s="52"/>
+      <c r="G136" s="51"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="18"/>
@@ -2427,7 +2443,7 @@
       <c r="D137" s="18"/>
       <c r="E137" s="16"/>
       <c r="F137" s="7"/>
-      <c r="G137" s="52"/>
+      <c r="G137" s="51"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="18"/>
@@ -2436,7 +2452,7 @@
       <c r="D138" s="18"/>
       <c r="E138" s="16"/>
       <c r="F138" s="7"/>
-      <c r="G138" s="52"/>
+      <c r="G138" s="51"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="18"/>
@@ -2445,7 +2461,7 @@
       <c r="D139" s="18"/>
       <c r="E139" s="16"/>
       <c r="F139" s="7"/>
-      <c r="G139" s="52"/>
+      <c r="G139" s="51"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="18"/>
@@ -2454,7 +2470,7 @@
       <c r="D140" s="18"/>
       <c r="E140" s="16"/>
       <c r="F140" s="7"/>
-      <c r="G140" s="52"/>
+      <c r="G140" s="51"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="18"/>
@@ -2463,7 +2479,7 @@
       <c r="D141" s="18"/>
       <c r="E141" s="16"/>
       <c r="F141" s="7"/>
-      <c r="G141" s="52"/>
+      <c r="G141" s="51"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="18"/>
@@ -2472,7 +2488,7 @@
       <c r="D142" s="18"/>
       <c r="E142" s="16"/>
       <c r="F142" s="7"/>
-      <c r="G142" s="52"/>
+      <c r="G142" s="51"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="18"/>
@@ -2481,7 +2497,7 @@
       <c r="D143" s="18"/>
       <c r="E143" s="16"/>
       <c r="F143" s="7"/>
-      <c r="G143" s="52"/>
+      <c r="G143" s="51"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="18"/>
@@ -2490,7 +2506,7 @@
       <c r="D144" s="18"/>
       <c r="E144" s="16"/>
       <c r="F144" s="7"/>
-      <c r="G144" s="52"/>
+      <c r="G144" s="51"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="18"/>
@@ -2499,7 +2515,7 @@
       <c r="D145" s="18"/>
       <c r="E145" s="16"/>
       <c r="F145" s="7"/>
-      <c r="G145" s="52"/>
+      <c r="G145" s="51"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="18"/>
@@ -2508,7 +2524,7 @@
       <c r="D146" s="18"/>
       <c r="E146" s="16"/>
       <c r="F146" s="7"/>
-      <c r="G146" s="52"/>
+      <c r="G146" s="51"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="18"/>
@@ -2517,7 +2533,7 @@
       <c r="D147" s="18"/>
       <c r="E147" s="16"/>
       <c r="F147" s="7"/>
-      <c r="G147" s="52"/>
+      <c r="G147" s="51"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="18"/>
@@ -2526,7 +2542,7 @@
       <c r="D148" s="18"/>
       <c r="E148" s="16"/>
       <c r="F148" s="7"/>
-      <c r="G148" s="52"/>
+      <c r="G148" s="51"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="18"/>
@@ -2535,7 +2551,7 @@
       <c r="D149" s="18"/>
       <c r="E149" s="16"/>
       <c r="F149" s="7"/>
-      <c r="G149" s="52"/>
+      <c r="G149" s="51"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="18"/>
@@ -2544,7 +2560,7 @@
       <c r="D150" s="18"/>
       <c r="E150" s="16"/>
       <c r="F150" s="7"/>
-      <c r="G150" s="52"/>
+      <c r="G150" s="51"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="18"/>
@@ -2553,7 +2569,7 @@
       <c r="D151" s="18"/>
       <c r="E151" s="16"/>
       <c r="F151" s="7"/>
-      <c r="G151" s="52"/>
+      <c r="G151" s="51"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="18"/>
@@ -2562,7 +2578,7 @@
       <c r="D152" s="18"/>
       <c r="E152" s="16"/>
       <c r="F152" s="7"/>
-      <c r="G152" s="52"/>
+      <c r="G152" s="51"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="18"/>
@@ -2571,7 +2587,7 @@
       <c r="D153" s="18"/>
       <c r="E153" s="16"/>
       <c r="F153" s="7"/>
-      <c r="G153" s="52"/>
+      <c r="G153" s="51"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="18"/>
@@ -2580,7 +2596,7 @@
       <c r="D154" s="18"/>
       <c r="E154" s="16"/>
       <c r="F154" s="7"/>
-      <c r="G154" s="52"/>
+      <c r="G154" s="51"/>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="18"/>
@@ -2589,7 +2605,7 @@
       <c r="D155" s="18"/>
       <c r="E155" s="16"/>
       <c r="F155" s="7"/>
-      <c r="G155" s="52"/>
+      <c r="G155" s="51"/>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="18"/>
@@ -2598,7 +2614,7 @@
       <c r="D156" s="18"/>
       <c r="E156" s="16"/>
       <c r="F156" s="7"/>
-      <c r="G156" s="52"/>
+      <c r="G156" s="51"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="18"/>
@@ -2607,7 +2623,7 @@
       <c r="D157" s="18"/>
       <c r="E157" s="16"/>
       <c r="F157" s="7"/>
-      <c r="G157" s="52"/>
+      <c r="G157" s="51"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="18"/>
@@ -2616,7 +2632,7 @@
       <c r="D158" s="18"/>
       <c r="E158" s="16"/>
       <c r="F158" s="7"/>
-      <c r="G158" s="52"/>
+      <c r="G158" s="51"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="18"/>
@@ -2625,7 +2641,7 @@
       <c r="D159" s="18"/>
       <c r="E159" s="16"/>
       <c r="F159" s="7"/>
-      <c r="G159" s="52"/>
+      <c r="G159" s="51"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="18"/>
@@ -2634,7 +2650,7 @@
       <c r="D160" s="18"/>
       <c r="E160" s="16"/>
       <c r="F160" s="7"/>
-      <c r="G160" s="52"/>
+      <c r="G160" s="51"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="18"/>
@@ -2643,7 +2659,7 @@
       <c r="D161" s="18"/>
       <c r="E161" s="16"/>
       <c r="F161" s="7"/>
-      <c r="G161" s="52"/>
+      <c r="G161" s="51"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="18"/>
@@ -2652,7 +2668,7 @@
       <c r="D162" s="18"/>
       <c r="E162" s="16"/>
       <c r="F162" s="7"/>
-      <c r="G162" s="52"/>
+      <c r="G162" s="51"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="18"/>
@@ -2661,7 +2677,7 @@
       <c r="D163" s="18"/>
       <c r="E163" s="16"/>
       <c r="F163" s="7"/>
-      <c r="G163" s="52"/>
+      <c r="G163" s="51"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="18"/>
@@ -2670,7 +2686,7 @@
       <c r="D164" s="18"/>
       <c r="E164" s="16"/>
       <c r="F164" s="7"/>
-      <c r="G164" s="52"/>
+      <c r="G164" s="51"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="18"/>
@@ -2679,7 +2695,7 @@
       <c r="D165" s="18"/>
       <c r="E165" s="16"/>
       <c r="F165" s="7"/>
-      <c r="G165" s="52"/>
+      <c r="G165" s="51"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="18"/>
@@ -2688,7 +2704,7 @@
       <c r="D166" s="18"/>
       <c r="E166" s="16"/>
       <c r="F166" s="7"/>
-      <c r="G166" s="52"/>
+      <c r="G166" s="51"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="18"/>
@@ -2697,7 +2713,7 @@
       <c r="D167" s="18"/>
       <c r="E167" s="16"/>
       <c r="F167" s="7"/>
-      <c r="G167" s="52"/>
+      <c r="G167" s="51"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="18"/>
@@ -2706,7 +2722,7 @@
       <c r="D168" s="18"/>
       <c r="E168" s="16"/>
       <c r="F168" s="7"/>
-      <c r="G168" s="52"/>
+      <c r="G168" s="51"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="18"/>
@@ -2715,7 +2731,7 @@
       <c r="D169" s="18"/>
       <c r="E169" s="16"/>
       <c r="F169" s="7"/>
-      <c r="G169" s="52"/>
+      <c r="G169" s="51"/>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="18"/>
@@ -2724,7 +2740,7 @@
       <c r="D170" s="18"/>
       <c r="E170" s="16"/>
       <c r="F170" s="7"/>
-      <c r="G170" s="52"/>
+      <c r="G170" s="51"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="18"/>
@@ -2733,7 +2749,7 @@
       <c r="D171" s="18"/>
       <c r="E171" s="16"/>
       <c r="F171" s="7"/>
-      <c r="G171" s="52"/>
+      <c r="G171" s="51"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="18"/>
@@ -2742,7 +2758,7 @@
       <c r="D172" s="18"/>
       <c r="E172" s="16"/>
       <c r="F172" s="7"/>
-      <c r="G172" s="52"/>
+      <c r="G172" s="51"/>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="18"/>
@@ -2751,7 +2767,7 @@
       <c r="D173" s="18"/>
       <c r="E173" s="16"/>
       <c r="F173" s="7"/>
-      <c r="G173" s="52"/>
+      <c r="G173" s="51"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="18"/>
@@ -2760,7 +2776,7 @@
       <c r="D174" s="18"/>
       <c r="E174" s="16"/>
       <c r="F174" s="7"/>
-      <c r="G174" s="52"/>
+      <c r="G174" s="51"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="18"/>
@@ -2769,7 +2785,7 @@
       <c r="D175" s="18"/>
       <c r="E175" s="16"/>
       <c r="F175" s="7"/>
-      <c r="G175" s="52"/>
+      <c r="G175" s="51"/>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="18"/>
@@ -2778,7 +2794,7 @@
       <c r="D176" s="18"/>
       <c r="E176" s="16"/>
       <c r="F176" s="7"/>
-      <c r="G176" s="52"/>
+      <c r="G176" s="51"/>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="18"/>
@@ -2787,7 +2803,7 @@
       <c r="D177" s="18"/>
       <c r="E177" s="16"/>
       <c r="F177" s="7"/>
-      <c r="G177" s="52"/>
+      <c r="G177" s="51"/>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="18"/>
@@ -2796,7 +2812,7 @@
       <c r="D178" s="18"/>
       <c r="E178" s="16"/>
       <c r="F178" s="7"/>
-      <c r="G178" s="52"/>
+      <c r="G178" s="51"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="18"/>
@@ -2805,7 +2821,7 @@
       <c r="D179" s="18"/>
       <c r="E179" s="16"/>
       <c r="F179" s="7"/>
-      <c r="G179" s="52"/>
+      <c r="G179" s="51"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="18"/>
@@ -2814,7 +2830,7 @@
       <c r="D180" s="18"/>
       <c r="E180" s="16"/>
       <c r="F180" s="7"/>
-      <c r="G180" s="52"/>
+      <c r="G180" s="51"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="18"/>
@@ -2823,7 +2839,7 @@
       <c r="D181" s="18"/>
       <c r="E181" s="16"/>
       <c r="F181" s="7"/>
-      <c r="G181" s="52"/>
+      <c r="G181" s="51"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="18"/>
@@ -2832,10 +2848,24 @@
       <c r="D182" s="18"/>
       <c r="E182" s="16"/>
       <c r="F182" s="7"/>
-      <c r="G182" s="52"/>
+      <c r="G182" s="51"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="18"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="18"/>
+      <c r="D183" s="18"/>
+      <c r="E183" s="16"/>
+      <c r="F183" s="7"/>
+      <c r="G183" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A11:C11">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D$11=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.78740157480314965" header="0.11811023622047245" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2850,18 +2880,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K182"/>
+  <sheetPr codeName="Feuil2"/>
+  <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="2.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
@@ -2885,10 +2916,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H3" s="20"/>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="52" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2915,7 +2946,7 @@
       <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="61"/>
       <c r="I6" s="11" t="s">
         <v>54</v>
       </c>
@@ -2930,7 +2961,7 @@
       <c r="C7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="61"/>
+      <c r="D7" s="60"/>
       <c r="I7" s="11" t="s">
         <v>56</v>
       </c>
@@ -2944,10 +2975,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="52" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2985,104 +3016,105 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+    </row>
+    <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B13" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="45" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G13" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="18"/>
+    <row r="14" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="59"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
       <c r="E15" s="16"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
+    </row>
+    <row r="16" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="54"/>
-    </row>
-    <row r="17" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="16"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="54"/>
-    </row>
-    <row r="18" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
+      <c r="H17" s="53"/>
+    </row>
+    <row r="18" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="59"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="16"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="54"/>
-    </row>
-    <row r="19" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60"/>
+      <c r="H18" s="53"/>
+    </row>
+    <row r="19" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="59"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="E19" s="16"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="55"/>
-    </row>
-    <row r="20" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60"/>
+      <c r="H19" s="53"/>
+    </row>
+    <row r="20" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -3091,28 +3123,28 @@
       <c r="G20" s="7"/>
       <c r="H20" s="54"/>
     </row>
-    <row r="21" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60"/>
+    <row r="21" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="59"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="16"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="54"/>
-    </row>
-    <row r="22" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
+      <c r="H21" s="53"/>
+    </row>
+    <row r="22" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="59"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
       <c r="E22" s="16"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="55"/>
-    </row>
-    <row r="23" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60"/>
+      <c r="H22" s="53"/>
+    </row>
+    <row r="23" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="59"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -3121,18 +3153,18 @@
       <c r="G23" s="7"/>
       <c r="H23" s="54"/>
     </row>
-    <row r="24" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60"/>
+    <row r="24" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="59"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="16"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="55"/>
-    </row>
-    <row r="25" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
+      <c r="H24" s="53"/>
+    </row>
+    <row r="25" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="59"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -3141,27 +3173,28 @@
       <c r="G25" s="7"/>
       <c r="H25" s="54"/>
     </row>
-    <row r="26" spans="1:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+    <row r="26" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="59"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="16"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="50"/>
-    </row>
-    <row r="27" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
+      <c r="H26" s="53"/>
+    </row>
+    <row r="27" spans="1:8" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="59"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="16"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
+      <c r="H27" s="49"/>
+    </row>
+    <row r="28" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="59"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -3169,8 +3202,8 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="60"/>
+    <row r="29" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="59"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -3178,97 +3211,96 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60"/>
+    <row r="30" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="59"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="16"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="56"/>
-    </row>
-    <row r="31" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
+    </row>
+    <row r="31" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="59"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="16"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="56"/>
-    </row>
-    <row r="32" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="60"/>
+      <c r="H31" s="55"/>
+    </row>
+    <row r="32" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="59"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
       <c r="E32" s="16"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="56"/>
-    </row>
-    <row r="33" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="60"/>
+      <c r="H32" s="55"/>
+    </row>
+    <row r="33" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="59"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="16"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="56"/>
-    </row>
-    <row r="34" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
+      <c r="H33" s="55"/>
+    </row>
+    <row r="34" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="59"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
       <c r="E34" s="16"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="56"/>
-    </row>
-    <row r="35" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
+      <c r="H34" s="55"/>
+    </row>
+    <row r="35" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="59"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="16"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="56"/>
-    </row>
-    <row r="36" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="60"/>
+      <c r="H35" s="55"/>
+    </row>
+    <row r="36" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="59"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
       <c r="E36" s="16"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="56"/>
-    </row>
-    <row r="37" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
+      <c r="H36" s="55"/>
+    </row>
+    <row r="37" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="59"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="16"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="56"/>
-    </row>
-    <row r="38" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+      <c r="H37" s="55"/>
+    </row>
+    <row r="38" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="59"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
       <c r="E38" s="16"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="56"/>
-    </row>
-    <row r="39" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="55"/>
+    </row>
+    <row r="39" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -3276,9 +3308,9 @@
       <c r="E39" s="16"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="56"/>
-    </row>
-    <row r="40" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H39" s="55"/>
+    </row>
+    <row r="40" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -3286,9 +3318,9 @@
       <c r="E40" s="16"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="56"/>
-    </row>
-    <row r="41" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H40" s="55"/>
+    </row>
+    <row r="41" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -3296,9 +3328,9 @@
       <c r="E41" s="16"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="54"/>
-    </row>
-    <row r="42" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H41" s="55"/>
+    </row>
+    <row r="42" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -3306,9 +3338,9 @@
       <c r="E42" s="16"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="54"/>
-    </row>
-    <row r="43" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H42" s="53"/>
+    </row>
+    <row r="43" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -3316,9 +3348,9 @@
       <c r="E43" s="16"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="57"/>
-    </row>
-    <row r="44" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H43" s="53"/>
+    </row>
+    <row r="44" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
@@ -3326,9 +3358,9 @@
       <c r="E44" s="16"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="54"/>
-    </row>
-    <row r="45" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H44" s="56"/>
+    </row>
+    <row r="45" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -3336,9 +3368,9 @@
       <c r="E45" s="16"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="57"/>
-    </row>
-    <row r="46" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H45" s="53"/>
+    </row>
+    <row r="46" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -3346,9 +3378,9 @@
       <c r="E46" s="16"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="57"/>
-    </row>
-    <row r="47" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H46" s="56"/>
+    </row>
+    <row r="47" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -3356,9 +3388,9 @@
       <c r="E47" s="16"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="57"/>
-    </row>
-    <row r="48" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H47" s="56"/>
+    </row>
+    <row r="48" spans="1:8" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
@@ -3366,10 +3398,9 @@
       <c r="E48" s="16"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="50"/>
-    </row>
-    <row r="49" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="56"/>
+    </row>
+    <row r="49" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
@@ -3378,8 +3409,9 @@
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="57"/>
-    </row>
-    <row r="50" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="49"/>
+    </row>
+    <row r="50" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -3387,10 +3419,9 @@
       <c r="E50" s="16"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="59"/>
-    </row>
-    <row r="51" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H50" s="56"/>
+    </row>
+    <row r="51" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -3398,9 +3429,10 @@
       <c r="E51" s="16"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="57"/>
-    </row>
-    <row r="52" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="56"/>
+      <c r="I51" s="58"/>
+    </row>
+    <row r="52" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -3408,9 +3440,9 @@
       <c r="E52" s="16"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="57"/>
-    </row>
-    <row r="53" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H52" s="56"/>
+    </row>
+    <row r="53" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -3418,9 +3450,9 @@
       <c r="E53" s="16"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="57"/>
-    </row>
-    <row r="54" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="56"/>
+    </row>
+    <row r="54" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -3428,10 +3460,9 @@
       <c r="E54" s="16"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="50"/>
-    </row>
-    <row r="55" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H54" s="56"/>
+    </row>
+    <row r="55" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -3439,10 +3470,10 @@
       <c r="E55" s="16"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="50"/>
-    </row>
-    <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H55" s="57"/>
+      <c r="I55" s="49"/>
+    </row>
+    <row r="56" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
@@ -3451,9 +3482,9 @@
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="57"/>
-      <c r="I56" s="59"/>
-    </row>
-    <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I56" s="49"/>
+    </row>
+    <row r="57" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -3461,10 +3492,10 @@
       <c r="E57" s="16"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
-      <c r="H57" s="57"/>
-      <c r="I57" s="59"/>
-    </row>
-    <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H57" s="56"/>
+      <c r="I57" s="58"/>
+    </row>
+    <row r="58" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
@@ -3472,9 +3503,10 @@
       <c r="E58" s="16"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="57"/>
-    </row>
-    <row r="59" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H58" s="56"/>
+      <c r="I58" s="58"/>
+    </row>
+    <row r="59" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
@@ -3482,9 +3514,9 @@
       <c r="E59" s="16"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="57"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H59" s="56"/>
+    </row>
+    <row r="60" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="18"/>
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
@@ -3492,6 +3524,7 @@
       <c r="E60" s="16"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
+      <c r="H60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="18"/>
@@ -3729,7 +3762,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
+      <c r="B87" s="18"/>
       <c r="C87" s="18"/>
       <c r="D87" s="18"/>
       <c r="E87" s="16"/>
@@ -4591,7 +4624,21 @@
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
     </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" s="18"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="18"/>
+      <c r="D183" s="18"/>
+      <c r="E183" s="16"/>
+      <c r="F183" s="7"/>
+      <c r="G183" s="7"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A11:C11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$D$11=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.78740157480314965" header="0.11811023622047245" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4606,6 +4653,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Feuil3"/>
   <dimension ref="A4:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>